<commit_message>
update from mstp meetings today
</commit_message>
<xml_diff>
--- a/utah connection emails.xlsx
+++ b/utah connection emails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UVUStudentLoaner\Desktop\pbischoff3.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10768192\Desktop\pbischoff3.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C588BC-DAB9-4E45-A217-9F1B384A4398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050C9569-A81D-4575-A5B3-8ED06676B860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26385" yWindow="2400" windowWidth="17250" windowHeight="8865" xr2:uid="{AEE92DA6-7BD3-460C-AFB8-186001E14C7C}"/>
+    <workbookView xWindow="31260" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{AEE92DA6-7BD3-460C-AFB8-186001E14C7C}"/>
   </bookViews>
   <sheets>
     <sheet name="contact info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>10. Are there any resources or opportunities that you would recommend for someone preparing to apply for an MD/PhD program?</t>
+  </si>
+  <si>
+    <t>very offputting. Almost rude</t>
+  </si>
+  <si>
+    <t>super kind, invested in my future. Email about age</t>
   </si>
 </sst>
 </file>
@@ -719,20 +725,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D6CA5E-AB1F-40DE-9E28-C02A75D0E4D1}">
-  <dimension ref="B2:F29"/>
+  <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -742,14 +750,14 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -759,11 +767,11 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -774,10 +782,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -787,11 +798,11 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -801,11 +812,11 @@
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -815,14 +826,14 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -832,11 +843,11 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -846,11 +857,11 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -860,11 +871,11 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -874,11 +885,11 @@
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
@@ -888,11 +899,11 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
@@ -902,11 +913,11 @@
       <c r="D13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -916,11 +927,11 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
@@ -930,11 +941,11 @@
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
@@ -944,14 +955,14 @@
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>49</v>
       </c>
@@ -961,11 +972,11 @@
       <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>52</v>
       </c>
@@ -976,7 +987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>54</v>
       </c>
@@ -986,11 +997,11 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1000,11 +1011,11 @@
       <c r="D20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
@@ -1014,11 +1025,11 @@
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1028,11 +1039,11 @@
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>65</v>
       </c>
@@ -1042,14 +1053,14 @@
       <c r="D23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>69</v>
       </c>
@@ -1059,14 +1070,14 @@
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
@@ -1076,11 +1087,11 @@
       <c r="D25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>76</v>
       </c>
@@ -1090,11 +1101,11 @@
       <c r="D26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>78</v>
       </c>
@@ -1104,11 +1115,11 @@
       <c r="D27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>81</v>
       </c>
@@ -1119,13 +1130,16 @@
         <v>83</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>86</v>
       </c>
@@ -1135,14 +1149,14 @@
       <c r="D29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" xr:uid="{2357EC4B-DEE0-4CDD-A620-A239A5436DDD}"/>
-    <hyperlink ref="E12" r:id="rId2" xr:uid="{61C64842-949F-46CF-8B54-74996D9F5673}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{2357EC4B-DEE0-4CDD-A620-A239A5436DDD}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{61C64842-949F-46CF-8B54-74996D9F5673}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -1157,59 +1171,60 @@
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>